<commit_message>
added method to get count of client by client manager
</commit_message>
<xml_diff>
--- a/src/test/java/ru/fds/tavrzcms3/testdata/encumbrance_new.xlsx
+++ b/src/test/java/ru/fds/tavrzcms3/testdata/encumbrance_new.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,9 +45,6 @@
     <t>Имя 1</t>
   </si>
   <si>
-    <t>PLEDGE</t>
-  </si>
-  <si>
     <t>номер 1</t>
   </si>
   <si>
@@ -70,12 +67,15 @@
   </si>
   <si>
     <t>в пользу кого 3</t>
+  </si>
+  <si>
+    <t>PLEDGE_OUR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,7 +391,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,15 +402,15 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -444,10 +444,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
         <v>40461</v>
@@ -456,7 +456,7 @@
         <v>40492</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -464,13 +464,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
         <v>40858</v>
@@ -479,7 +479,7 @@
         <v>40888</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -487,13 +487,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="2">
         <v>40858</v>
@@ -502,7 +502,7 @@
         <v>40888</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>